<commit_message>
Cleared error, working perfectly
</commit_message>
<xml_diff>
--- a/transactions2.xlsx
+++ b/transactions2.xlsx
@@ -478,7 +478,6 @@
           <t xml:space="preserve">price </t>
         </is>
       </c>
-      <c r="D1" t="inlineStr"/>
     </row>
     <row r="2" ht="12.8" customHeight="1" s="3">
       <c r="A2" s="2" t="n">
@@ -491,7 +490,7 @@
         <v>5.95</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>5.355</v>
       </c>
     </row>
     <row r="3" ht="12.8" customHeight="1" s="3">
@@ -505,7 +504,7 @@
         <v>6.95</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>6.255</v>
       </c>
     </row>
     <row r="4" ht="12.8" customHeight="1" s="3">
@@ -519,7 +518,7 @@
         <v>7.95</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>7.155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>